<commit_message>
Add missing matches log to landing_page.py
</commit_message>
<xml_diff>
--- a/NPLQ fixtures.xlsx
+++ b/NPLQ fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3587EE-3BA4-4FC1-8A4B-30B2D5AA1F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28CCEE0-993B-4633-8D75-325BA14610DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{502D6ED2-73F8-4C19-A642-B7CB9A006B4C}"/>
   </bookViews>
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add data of SCW vs Redlands match (round 8)
</commit_message>
<xml_diff>
--- a/NPLQ fixtures.xlsx
+++ b/NPLQ fixtures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n10637427\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BBCA10-5EA7-4CD7-8390-E0E1C2175B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FBB973-03E7-42A5-B550-DC71219987E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{502D6ED2-73F8-4C19-A642-B7CB9A006B4C}"/>
+    <workbookView xWindow="3450" yWindow="10470" windowWidth="21600" windowHeight="11385" xr2:uid="{502D6ED2-73F8-4C19-A642-B7CB9A006B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="NPLQ fixtures" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -528,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB2F058-46A0-47E5-B2BA-3739D028E3CF}">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1961,7 +1960,7 @@
         <v>3</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -1978,7 +1977,7 @@
         <v>31</v>
       </c>
       <c r="E50" s="2">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>34</v>
@@ -1987,7 +1986,7 @@
         <v>13</v>
       </c>
       <c r="H50" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>28</v>
@@ -2007,7 +2006,7 @@
         <v>15</v>
       </c>
       <c r="E51" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>8</v>
@@ -2016,7 +2015,7 @@
         <v>9</v>
       </c>
       <c r="H51" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>28</v>
@@ -2036,7 +2035,7 @@
         <v>17</v>
       </c>
       <c r="E52" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>22</v>
@@ -2045,7 +2044,7 @@
         <v>23</v>
       </c>
       <c r="H52" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>28</v>
@@ -2065,7 +2064,7 @@
         <v>11</v>
       </c>
       <c r="E53" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>32</v>
@@ -2074,7 +2073,7 @@
         <v>33</v>
       </c>
       <c r="H53" s="2">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>28</v>
@@ -2094,7 +2093,7 @@
         <v>19</v>
       </c>
       <c r="E54" s="2">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>26</v>
@@ -2103,7 +2102,7 @@
         <v>27</v>
       </c>
       <c r="H54" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>28</v>
@@ -2123,7 +2122,7 @@
         <v>25</v>
       </c>
       <c r="E55" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>20</v>
@@ -2132,7 +2131,7 @@
         <v>21</v>
       </c>
       <c r="H55" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Added data for round 10
</commit_message>
<xml_diff>
--- a/NPLQ fixtures.xlsx
+++ b/NPLQ fixtures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n10637427\Documents\GitHub\olympicdataapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FBB973-03E7-42A5-B550-DC71219987E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD47A2C-3EFB-45B2-986E-BBC653E385D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="10470" windowWidth="21600" windowHeight="11385" xr2:uid="{502D6ED2-73F8-4C19-A642-B7CB9A006B4C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{502D6ED2-73F8-4C19-A642-B7CB9A006B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="NPLQ fixtures" sheetId="1" r:id="rId1"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB2F058-46A0-47E5-B2BA-3739D028E3CF}">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2151,7 +2151,7 @@
         <v>11</v>
       </c>
       <c r="E56" s="2">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>20</v>
@@ -2160,10 +2160,10 @@
         <v>21</v>
       </c>
       <c r="H56" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2180,7 +2180,7 @@
         <v>9</v>
       </c>
       <c r="E57" s="2">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>18</v>
@@ -2189,10 +2189,10 @@
         <v>19</v>
       </c>
       <c r="H57" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2209,7 +2209,7 @@
         <v>31</v>
       </c>
       <c r="E58" s="2">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>24</v>
@@ -2218,10 +2218,10 @@
         <v>25</v>
       </c>
       <c r="H58" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2238,7 +2238,7 @@
         <v>27</v>
       </c>
       <c r="E59" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>32</v>
@@ -2247,10 +2247,10 @@
         <v>33</v>
       </c>
       <c r="H59" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2267,7 +2267,7 @@
         <v>17</v>
       </c>
       <c r="E60" s="2">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>14</v>
@@ -2276,10 +2276,10 @@
         <v>15</v>
       </c>
       <c r="H60" s="2">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
         <v>13</v>
       </c>
       <c r="E61" s="2">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>22</v>
@@ -2305,7 +2305,7 @@
         <v>23</v>
       </c>
       <c r="H61" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>28</v>

</xml_diff>